<commit_message>
feat: integrate YouTubeAPIClient and update song model to include YouTube link
</commit_message>
<xml_diff>
--- a/genius_songs.xlsx
+++ b/genius_songs.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,8 @@
     <col width="30" customWidth="1" min="3" max="3"/>
     <col width="80" customWidth="1" min="4" max="4"/>
     <col width="50" customWidth="1" min="5" max="5"/>
-    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="50" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -471,6 +472,11 @@
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>enlace_youtube</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>discografica</t>
         </is>
@@ -601,6 +607,11 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=SEjw5rdyvVg</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -682,6 +693,11 @@
         </is>
       </c>
       <c r="F3" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QFs3PIZb3js</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -768,6 +784,11 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=8iPcqtHoR3U</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -848,6 +869,11 @@
         </is>
       </c>
       <c r="F5" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=0XCot42qTvA</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -963,6 +989,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=XlmaJ-yU46U</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -1061,6 +1092,11 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=jk4HYngf65w</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -1158,6 +1194,11 @@
         </is>
       </c>
       <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=TarQP-rtabI</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1242,6 +1283,11 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=ElU-VcWEhRU</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -1366,6 +1412,11 @@
         </is>
       </c>
       <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=z2pt4CN4rhc</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1450,6 +1501,11 @@
         </is>
       </c>
       <c r="F11" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=GHLVjriwzFg</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1548,6 +1604,11 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=CsziEW_gYhU</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -1613,6 +1674,11 @@
         </is>
       </c>
       <c r="F13" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=b_HDhkw6g7I</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1693,6 +1759,11 @@
         </is>
       </c>
       <c r="F14" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=4eCL0l9iD5A</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1790,6 +1861,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=elGZbcpGzdU</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -1862,6 +1938,11 @@
         </is>
       </c>
       <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Hz9lhqxl_gQ</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -1967,6 +2048,11 @@
         </is>
       </c>
       <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=RjMWh1vve6E</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2081,6 +2167,11 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=RSRzIrOqaN4</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2164,6 +2255,11 @@
         </is>
       </c>
       <c r="F19" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=hPT2FGoSOr8</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2268,6 +2364,11 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=uPCZm2Tvjpo</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2337,6 +2438,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=kADoBrj4934</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2405,6 +2511,11 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=2LiZyAIVmbs</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2472,6 +2583,11 @@
         </is>
       </c>
       <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=sxbKoqz9bNM</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2575,6 +2691,11 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=gxWexyncaTs</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2633,6 +2754,11 @@
         </is>
       </c>
       <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=LakJahiBl2Y</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2707,6 +2833,11 @@
         </is>
       </c>
       <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=zHhza3EgHe8</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2803,6 +2934,11 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=suQC8d-YkeU</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -2866,6 +3002,11 @@
         </is>
       </c>
       <c r="F28" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QSCVVYd1y7Q</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -2939,6 +3080,11 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=Es6yYN0iEj4</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3004,6 +3150,11 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=8XD1ZdUJKkk</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3066,6 +3217,11 @@
         </is>
       </c>
       <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=8Ei86cJIWlk</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3144,6 +3300,11 @@
         </is>
       </c>
       <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=glVFC1G86zA</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3253,6 +3414,11 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=GfFnQ2l2FxM</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3344,6 +3510,11 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=MqlcnVaqS8I</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3422,6 +3593,11 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=tYLJRRRqiLI</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3491,6 +3667,11 @@
         </is>
       </c>
       <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=WC94NQnW3_s</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3579,6 +3760,11 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=0m5SXO8qK78</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3656,6 +3842,11 @@
         </is>
       </c>
       <c r="F38" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=HPvpJcR6ICc</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3754,6 +3945,11 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=BVBZBpfWtp0</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3813,6 +4009,11 @@
         </is>
       </c>
       <c r="F40" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ePtOXORN96A</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -3883,6 +4084,11 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=EMRaPVzlqyA</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -3950,6 +4156,11 @@
         </is>
       </c>
       <c r="F42" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Vvg6GYgiq9Q</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4031,6 +4242,11 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=APhN7FHPcnw</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4098,6 +4314,11 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=r4kJ2o_6ouM</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4158,6 +4379,11 @@
         </is>
       </c>
       <c r="F45" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=tuV_1NKnQxY</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4220,6 +4446,11 @@
         </is>
       </c>
       <c r="F46" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=q79vUDskBGQ</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4302,6 +4533,11 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=5oMZic5Ba0g</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4370,6 +4606,11 @@
         </is>
       </c>
       <c r="F48" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=VY5zYtdhOCI</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4442,6 +4683,11 @@
         </is>
       </c>
       <c r="F49" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=HuealJ5miJA</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4525,6 +4771,11 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=nZFJmyC8lq4</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4591,6 +4842,11 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=ZlOupl2eaEA</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4688,6 +4944,11 @@
         </is>
       </c>
       <c r="F52" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=_4NBD3SqBwg</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4760,6 +5021,11 @@
         </is>
       </c>
       <c r="F53" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=v0ckuv1xBm0</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -4869,6 +5135,11 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=LvgEpio1-kA</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -4936,6 +5207,11 @@
         </is>
       </c>
       <c r="F55" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=daZ2aRW7ico</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5028,6 +5304,11 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=SRLRCCffvlA</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -5099,6 +5380,11 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=qYo68mjl6N8</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -5154,6 +5440,11 @@
         </is>
       </c>
       <c r="F58" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=sEZ71GJwzZg</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5217,6 +5508,11 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=NGTxYqu7xsg</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -5277,6 +5573,11 @@
         </is>
       </c>
       <c r="F60" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=d_O2GR5xvFk</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5350,6 +5651,11 @@
         </is>
       </c>
       <c r="F61" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Tzaxx2kEWPM</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5424,6 +5730,11 @@
         </is>
       </c>
       <c r="F62" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=9ynXEZ9QC08</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5507,6 +5818,11 @@
         </is>
       </c>
       <c r="F63" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=S51xo-295BY</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -5612,6 +5928,11 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=cG9EcD72_es</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -5680,6 +6001,11 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
+          <t>https://www.youtube.com/watch?v=kgc6GxptSg4</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
           <t>N/A</t>
         </is>
       </c>
@@ -5697,10 +6023,84 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t>Mujer Interesada</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">1 Contributor
+Mujer Interesada Lyrics
+Cuando te ofrecia yo mi amor
+Tu no me quisiste aceptar
+Andaba como un loco por ti
+Tu gozabas al verme sufrir
+Entonces busqu otro amor
+Y a ti ya te olvid
+Mira, ya no me busques mas
+Como amor ya no te puedo ver
+Ay no quiero nada contigo
+No me interesa tu amor 
+Como voy amar a una mujer
+Que divide el amor y el inters
+Cuando mi vida est en flor
+Sera mio todito su amor
+Y si vuelvo a ser pobre otra vez
+No tendr dinero tampoco mujer
+Ay
+No quiero nada contigo
+No me interesa tu amor 
+Ay que yo era quin te gustaba entre los hombres
+Que querian ser dueos de ti
+Y por ser pobre demas
+Mis palabras no querias escuchar
+Mas tarde a mi Dios me ayud
+Y andabas buscando mi amor
+Ay
+Ya no quiero nada contigo
+No me interesa tu amor 
+No puedo negar que eres bonita
+Y que tienes encantospor de mas
+Pero no sientes amor
+Solo piensas en la vanidad
+Ay mujer interesada
+Vete aljate de mi
+Ya no quiero nada contigo
+No me interesa tu amor </t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>https://genius.com/Zacarias-ferreira-mujer-interesada-lyrics</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=VFZso5izLRc</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Zacarías Ferreira</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>Chica De Mi Barrio</t>
         </is>
       </c>
-      <c r="D66" s="2" t="inlineStr">
+      <c r="D67" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">2 Contributors
 Chica De Mi Barrio Lyrics
@@ -5736,34 +6136,39 @@
 Estoy esperandote </t>
         </is>
       </c>
-      <c r="E66" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>https://genius.com/Zacarias-ferreira-chica-de-mi-barrio-lyrics</t>
         </is>
       </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=sPC6ycHExg0</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>El Chaval de la Bachata</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="C68" t="inlineStr">
         <is>
           <t>Devuélveme Todo</t>
         </is>
       </c>
-      <c r="D67" s="2" t="inlineStr">
+      <c r="D68" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Devuélveme Todo Lyrics
@@ -5818,34 +6223,39 @@
 Lo que me pertenece</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>https://genius.com/El-chaval-de-la-bachata-devuelveme-todo-annotated</t>
         </is>
       </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=9rt8r9g63bk</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>Zacarías Ferreira</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>Te extraño</t>
         </is>
       </c>
-      <c r="D68" s="2" t="inlineStr">
+      <c r="D69" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Te extraño Lyrics
@@ -5880,34 +6290,39 @@
 No podría vivir sin ti, jamás</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>https://genius.com/Zacarias-ferreira-te-extrano-lyrics</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=A7RQIwtEuNM</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>Luis Vargas</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>Estoy Condenado</t>
         </is>
       </c>
-      <c r="D69" s="2" t="inlineStr">
+      <c r="D70" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Estoy Condenado Lyrics
@@ -5990,34 +6405,39 @@
 Dame más amor</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>https://genius.com/Luis-vargas-estoy-condenado-annotated</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=_s777yfsWRw</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>La Bilirrubina</t>
         </is>
       </c>
-      <c r="D70" s="2" t="inlineStr">
+      <c r="D71" s="2" t="inlineStr">
         <is>
           <t>7 Contributors
 La Bilirrubina Lyrics
@@ -6119,34 +6539,39 @@
 )</t>
         </is>
       </c>
-      <c r="E70" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-la-bilirrubina-lyrics</t>
         </is>
       </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=x3G4VFThbEg</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>A Pedir Su Mano</t>
         </is>
       </c>
-      <c r="D71" s="2" t="inlineStr">
+      <c r="D72" s="2" t="inlineStr">
         <is>
           <t>5 Contributors
 A Pedir Su Mano Lyrics
@@ -6217,34 +6642,39 @@
 Ioh</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-a-pedir-su-mano-lyrics</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=0lGBwSiStfE</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C73" t="inlineStr">
         <is>
           <t>Visa Para Un Sueño</t>
         </is>
       </c>
-      <c r="D72" s="2" t="inlineStr">
+      <c r="D73" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 Visa Para Un Sueño Lyrics
@@ -6295,34 +6725,39 @@
 Buscando visa para no volver</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-visa-para-un-sueno-lyrics</t>
         </is>
       </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=PZ1eWwi0NZA</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>El Niagara En Bicicleta</t>
         </is>
       </c>
-      <c r="D73" s="2" t="inlineStr">
+      <c r="D74" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 El Niagara En Bicicleta Lyrics
@@ -6406,34 +6841,39 @@
 No me digan que le está latiendo, oh no</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-el-niagara-en-bicicleta-lyrics</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=Ae6EQYHjN4M</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="C75" t="inlineStr">
         <is>
           <t>Ojalá Que Llueva Café</t>
         </is>
       </c>
-      <c r="D74" s="2" t="inlineStr">
+      <c r="D75" s="2" t="inlineStr">
         <is>
           <t>13 Contributors
 Ojalá Que Llueva Café Lyrics
@@ -6501,34 +6941,39 @@
 Ojalá que llueva café</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-ojala-que-llueva-cafe-lyrics</t>
         </is>
       </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=suQC8d-YkeU</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="C76" t="inlineStr">
         <is>
           <t>Rosalía</t>
         </is>
       </c>
-      <c r="D75" s="2" t="inlineStr">
+      <c r="D76" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 Rosalía Lyrics
@@ -6636,34 +7081,39 @@
 Rosalía</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr">
+      <c r="E76" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-rosalia-lyrics</t>
         </is>
       </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=81p_KumYYt8</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="C77" t="inlineStr">
         <is>
           <t>Woman Del Callao</t>
         </is>
       </c>
-      <c r="D76" s="2" t="inlineStr">
+      <c r="D77" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 Woman Del Callao Lyrics
@@ -6798,34 +7248,39 @@
 Tiene mucho tempo</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr">
+      <c r="E77" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-woman-del-callao-lyrics</t>
         </is>
       </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=kQgXAn5J7is</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
         <is>
           <t>Juan Luis Guerra</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="C78" t="inlineStr">
         <is>
           <t>La Cosquillita</t>
         </is>
       </c>
-      <c r="D77" s="2" t="inlineStr">
+      <c r="D78" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 La Cosquillita Lyrics
@@ -6894,34 +7349,39 @@
 Niña, ¡qué bien!</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr">
+      <c r="E78" t="inlineStr">
         <is>
           <t>https://genius.com/Juan-luis-guerra-la-cosquillita-lyrics</t>
         </is>
       </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=3SJwKBxKuoM</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
         <is>
           <t>Johnny Ventura</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>Patacón Pisao</t>
         </is>
       </c>
-      <c r="D78" s="2" t="inlineStr">
+      <c r="D79" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Patacón Pisao Lyrics
@@ -6965,34 +7425,39 @@
 Patacón pisaoPisao</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>https://genius.com/Johnny-ventura-patacon-pisao-lyrics</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=t9UO7jY0bcs</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
         <is>
           <t>Johnny Ventura</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>¿Pitaste?</t>
         </is>
       </c>
-      <c r="D79" s="2" t="inlineStr">
+      <c r="D80" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 ¿Pitaste? Lyrics
@@ -7038,34 +7503,39 @@
 Ese pito</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>https://genius.com/Johnny-ventura-pitaste-lyrics</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=i1BrB9PL-ng</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
         <is>
           <t>Fernando Villalona</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="C81" t="inlineStr">
         <is>
           <t>Tabaco Y Ron</t>
         </is>
       </c>
-      <c r="D80" s="2" t="inlineStr">
+      <c r="D81" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 Tabaco Y Ron Lyrics
@@ -7134,34 +7604,39 @@
 Para hablar de nuestras penas</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr">
+      <c r="E81" t="inlineStr">
         <is>
           <t>https://genius.com/Fernando-villalona-tabaco-y-ron-lyrics</t>
         </is>
       </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=r4l2VrWBQ0c</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>Madre Mia</t>
         </is>
       </c>
-      <c r="D81" s="2" t="inlineStr">
+      <c r="D82" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Madre Mia Lyrics
@@ -7187,34 +7662,39 @@
 No me llore mi viejita, confie en mi, usted sabe que yo no le fallo...</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-madre-mia-lyrics</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=MweR9bADIJI</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>La Ventanita</t>
         </is>
       </c>
-      <c r="D82" s="2" t="inlineStr">
+      <c r="D83" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 La Ventanita Lyrics
@@ -7269,34 +7749,39 @@
 Tengo el alma en pedazos</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="E83" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-la-ventanita-lyrics</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=TMnoDzBbvk0</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="C84" t="inlineStr">
         <is>
           <t>Vete Y Dile</t>
         </is>
       </c>
-      <c r="D83" s="2" t="inlineStr">
+      <c r="D84" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Vete Y Dile Lyrics
@@ -7383,34 +7868,39 @@
 Dile oite</t>
         </is>
       </c>
-      <c r="E83" t="inlineStr">
+      <c r="E84" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-vete-y-dile-lyrics</t>
         </is>
       </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=WbKHlXe14W8</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>Aquello Que Me Diste</t>
         </is>
       </c>
-      <c r="D84" s="2" t="inlineStr">
+      <c r="D85" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Aquello Que Me Diste Lyrics
@@ -7467,34 +7957,39 @@
 Y todo aquello que me diste</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-aquello-que-me-diste-lyrics</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ou2ddsB64z4</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
         <is>
           <t>Bonny Cepeda</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>Asesina</t>
         </is>
       </c>
-      <c r="D85" s="2" t="inlineStr">
+      <c r="D86" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 Asesina Lyrics
@@ -7543,34 +8038,39 @@
 Complacida no quedo</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E86" t="inlineStr">
         <is>
           <t>https://genius.com/Bonny-cepeda-asesina-lyrics</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=V1jnol6o1kQ</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
         <is>
           <t>Bonny Cepeda</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C87" t="inlineStr">
         <is>
           <t>Una Fotografia</t>
         </is>
       </c>
-      <c r="D86" s="2" t="inlineStr">
+      <c r="D87" s="2" t="inlineStr">
         <is>
           <t>6 Contributors
 Una Fotografia Lyrics
@@ -7617,34 +8117,39 @@
 Te llevo en mi mente a ti Ginet</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E87" t="inlineStr">
         <is>
           <t>https://genius.com/Bonny-cepeda-una-fotografia-lyrics</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=1crMUfqH6i0</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
         <is>
           <t>Bonny Cepeda</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>¡ay doctor!</t>
         </is>
       </c>
-      <c r="D87" s="2" t="inlineStr">
+      <c r="D88" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 ¡ay doctor! Lyrics
@@ -7701,34 +8206,39 @@
 Ay Ay Ay Doctor X 8</t>
         </is>
       </c>
-      <c r="E87" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>https://genius.com/Bonny-cepeda-ay-doctor-lyrics</t>
         </is>
       </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QfrnxJ4OQko</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
         <is>
           <t>Mala Fe</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C89" t="inlineStr">
         <is>
           <t>La Vaca</t>
         </is>
       </c>
-      <c r="D88" s="2" t="inlineStr">
+      <c r="D89" s="2" t="inlineStr">
         <is>
           <t>5 Contributors
 La Vaca Lyrics
@@ -7845,34 +8355,39 @@
 Musicos paguen que no han pagado</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="E89" t="inlineStr">
         <is>
           <t>https://genius.com/Mala-fe-la-vaca-lyrics</t>
         </is>
       </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=2Gow_mzRTO4</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
         <is>
           <t>Wilfrido Vargas</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="C90" t="inlineStr">
         <is>
           <t>El Baile del Perrito</t>
         </is>
       </c>
-      <c r="D89" s="2" t="inlineStr">
+      <c r="D90" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 El Baile del Perrito Lyrics
@@ -7940,34 +8455,39 @@
 El baile del perro ju!</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr">
+      <c r="E90" t="inlineStr">
         <is>
           <t>https://genius.com/Wilfrido-vargas-el-baile-del-perrito-lyrics</t>
         </is>
       </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=fs1Fg07CsQs</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
         <is>
           <t>Wilfrido Vargas</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="C91" t="inlineStr">
         <is>
           <t>Abusadora</t>
         </is>
       </c>
-      <c r="D90" s="2" t="inlineStr">
+      <c r="D91" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 Abusadora Lyrics
@@ -8099,34 +8619,39 @@
 Abusadora</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr">
+      <c r="E91" t="inlineStr">
         <is>
           <t>https://genius.com/Wilfrido-vargas-and-sandy-reyes-abusadora-lyrics</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QweFe4CeAJg</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
         <is>
           <t>Wilfrido Vargas</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>El Africano</t>
         </is>
       </c>
-      <c r="D91" s="2" t="inlineStr">
+      <c r="D92" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 El Africano Lyrics
@@ -8165,34 +8690,39 @@
 Que le den</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr">
+      <c r="E92" t="inlineStr">
         <is>
           <t>https://genius.com/Wilfrido-vargas-el-africano-lyrics</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=1DbXzlhKS5s</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
         <is>
           <t>Wilfrido Vargas</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="C93" t="inlineStr">
         <is>
           <t>El Jardinero</t>
         </is>
       </c>
-      <c r="D92" s="2" t="inlineStr">
+      <c r="D93" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 El Jardinero Lyrics
@@ -8339,44 +8869,17 @@
 )</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr">
+      <c r="E93" t="inlineStr">
         <is>
           <t>https://genius.com/Wilfrido-vargas-el-jardinero-lyrics</t>
         </is>
       </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Milly Quezada</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>Volvio Juanita</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>https://genius.com/Milly-quezada-volvio-juanita-lyrics</t>
-        </is>
-      </c>
       <c r="F93" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=8uJfGp8yjrg</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
@@ -8395,10 +8898,47 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
+          <t>Volvio Juanita</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>https://genius.com/Milly-quezada-volvio-juanita-lyrics</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=E6soE-1p3kw</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>Milly Quezada</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
           <t>De Colores</t>
         </is>
       </c>
-      <c r="D94" s="2" t="inlineStr">
+      <c r="D95" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 De Colores Lyrics
@@ -8453,34 +8993,39 @@
 Llenaste , llenaste , llenaste todo</t>
         </is>
       </c>
-      <c r="E94" t="inlineStr">
+      <c r="E95" t="inlineStr">
         <is>
           <t>https://genius.com/Milly-quezada-de-colores-lyrics</t>
         </is>
       </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=-_fCguTGj88</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
         <is>
           <t>Milly Quezada,Los Vecinos</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="C96" t="inlineStr">
         <is>
           <t>La Guacherna</t>
         </is>
       </c>
-      <c r="D95" s="2" t="inlineStr">
+      <c r="D96" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 La Guacherna Lyrics
@@ -8527,34 +9072,39 @@
 Y nos vamos pa la guacherna!!</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr">
+      <c r="E96" t="inlineStr">
         <is>
           <t>https://genius.com/Milly-quezadalos-vecinos-la-guacherna-lyrics</t>
         </is>
       </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=6Nw3_rvV0Y0</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
         <is>
           <t>Rubby Pérez</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="C97" t="inlineStr">
         <is>
           <t>Buscando Tus Besos</t>
         </is>
       </c>
-      <c r="D96" s="2" t="inlineStr">
+      <c r="D97" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Buscando Tus Besos Lyrics
@@ -8593,34 +9143,39 @@
 Un ser extraño, sin amor</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr">
+      <c r="E97" t="inlineStr">
         <is>
           <t>https://genius.com/Rubby-perez-buscando-tus-besos-lyrics</t>
         </is>
       </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=mHwg8V9HwXM</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
         <is>
           <t>Los Hermanos Rosario</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="C98" t="inlineStr">
         <is>
           <t>La Dueña del Swing</t>
         </is>
       </c>
-      <c r="D97" s="2" t="inlineStr">
+      <c r="D98" s="2" t="inlineStr">
         <is>
           <t>5 Contributors
 La Dueña del Swing Lyrics
@@ -8724,34 +9279,39 @@
 Rosario</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr">
+      <c r="E98" t="inlineStr">
         <is>
           <t>https://genius.com/Los-hermanos-rosario-la-duena-del-swing-lyrics</t>
         </is>
       </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=QCcBiAwp9nc</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
         <is>
           <t>Los Hermanos Rosario</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="C99" t="inlineStr">
         <is>
           <t>Morena Ven</t>
         </is>
       </c>
-      <c r="D98" s="2" t="inlineStr">
+      <c r="D99" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Morena Ven Lyrics
@@ -8801,34 +9361,39 @@
 Agáchate...</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr">
+      <c r="E99" t="inlineStr">
         <is>
           <t>https://genius.com/Los-hermanos-rosario-morena-ven-annotated</t>
         </is>
       </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=NakaWu2BXa4</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
         <is>
           <t>Toño Rosario</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="C100" t="inlineStr">
         <is>
           <t>KULIKITAKA (En Vivo) / Mula (Mixed)</t>
         </is>
       </c>
-      <c r="D99" s="2" t="inlineStr">
+      <c r="D100" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 KULIKITAKA  / Mula  Lyrics
@@ -8843,34 +9408,39 @@
 When I see you dancing I'm like hola, hola, hola, hola</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr">
+      <c r="E100" t="inlineStr">
         <is>
           <t>https://genius.com/Tono-rosario-and-eliminate-kulikitaka-en-vivo-mula-mixed-lyrics</t>
         </is>
       </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
         <is>
           <t>Toño Rosario</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="C101" t="inlineStr">
         <is>
           <t>Alegria</t>
         </is>
       </c>
-      <c r="D100" s="2" t="inlineStr">
+      <c r="D101" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Alegria Lyrics
@@ -8919,34 +9489,39 @@
 Resistiré etc etc....</t>
         </is>
       </c>
-      <c r="E100" t="inlineStr">
+      <c r="E101" t="inlineStr">
         <is>
           <t>https://genius.com/Tono-rosario-alegria-lyrics</t>
         </is>
       </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=qQ5FEe4eTy0</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
         <is>
           <t>Eddy Herrera</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="C102" t="inlineStr">
         <is>
           <t>Pégame Tu Vicio</t>
         </is>
       </c>
-      <c r="D101" s="2" t="inlineStr">
+      <c r="D102" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 Pégame Tu Vicio Lyrics
@@ -9042,34 +9617,39 @@
 El vicio de tus labios</t>
         </is>
       </c>
-      <c r="E101" t="inlineStr">
+      <c r="E102" t="inlineStr">
         <is>
           <t>https://genius.com/Eddy-herrera-pegame-tu-vicio-lyrics</t>
         </is>
       </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=yWSQxGppcFA</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
         <is>
           <t>Eddy Herrera</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="C103" t="inlineStr">
         <is>
           <t>Tú Eres Ajena</t>
         </is>
       </c>
-      <c r="D102" s="2" t="inlineStr">
+      <c r="D103" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 Tú Eres Ajena Lyrics
@@ -9137,34 +9717,39 @@
 ¿Bailamos?</t>
         </is>
       </c>
-      <c r="E102" t="inlineStr">
+      <c r="E103" t="inlineStr">
         <is>
           <t>https://genius.com/Eddy-herrera-tu-eres-ajena-lyrics</t>
         </is>
       </c>
-      <c r="F102" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=uzU3x_egiEk</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
         <is>
           <t>Eddy Herrera</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="C104" t="inlineStr">
         <is>
           <t>Carolina</t>
         </is>
       </c>
-      <c r="D103" s="2" t="inlineStr">
+      <c r="D104" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Carolina Lyrics
@@ -9197,34 +9782,39 @@
 Só Carolina não viu</t>
         </is>
       </c>
-      <c r="E103" t="inlineStr">
+      <c r="E104" t="inlineStr">
         <is>
           <t>https://genius.com/Eddy-herrera-carolina-lyrics</t>
         </is>
       </c>
-      <c r="F103" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=eotdaHXYV3Y</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
         <is>
           <t>Eddy Herrera</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="C105" t="inlineStr">
         <is>
           <t>Demasiado Niña</t>
         </is>
       </c>
-      <c r="D104" s="2" t="inlineStr">
+      <c r="D105" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 Demasiado Niña Lyrics
@@ -9272,34 +9862,39 @@
 Mi amor  ?</t>
         </is>
       </c>
-      <c r="E104" t="inlineStr">
+      <c r="E105" t="inlineStr">
         <is>
           <t>https://genius.com/Eddy-herrera-demasiado-nina-lyrics</t>
         </is>
       </c>
-      <c r="F104" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=duhqF3c3ru0</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
         <is>
           <t>Hector Acosta “El Torito”</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
+      <c r="C106" t="inlineStr">
         <is>
           <t>Me Voy - Bachata</t>
         </is>
       </c>
-      <c r="D105" s="2" t="inlineStr">
+      <c r="D106" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 Me Voy - Bachata Lyrics
@@ -9335,34 +9930,39 @@
 Y tú ya no tendrás mi amor, amárgate escuchando esta canción</t>
         </is>
       </c>
-      <c r="E105" t="inlineStr">
+      <c r="E106" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-el-torito-me-voy-bachata-lyrics</t>
         </is>
       </c>
-      <c r="F105" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=rmerQRm3GJk</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
         <is>
           <t>Hector Acosta “El Torito”</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
+      <c r="C107" t="inlineStr">
         <is>
           <t>Sin Perdon</t>
         </is>
       </c>
-      <c r="D106" s="2" t="inlineStr">
+      <c r="D107" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Sin Perdon Lyrics
@@ -9409,34 +10009,39 @@
 ¡me dolió hasta el alma eso me llego!</t>
         </is>
       </c>
-      <c r="E106" t="inlineStr">
+      <c r="E107" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-el-torito-sin-perdon-lyrics</t>
         </is>
       </c>
-      <c r="F106" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ot6wDVHqVNw</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
         <is>
           <t>Hector Acosta “El Torito”</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
+      <c r="C108" t="inlineStr">
         <is>
           <t>Me Duele La Cabeza</t>
         </is>
       </c>
-      <c r="D107" s="2" t="inlineStr">
+      <c r="D108" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 Me Duele La Cabeza Lyrics
@@ -9499,34 +10104,39 @@
 Menos que te perdi</t>
         </is>
       </c>
-      <c r="E107" t="inlineStr">
+      <c r="E108" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-el-torito-me-duele-la-cabeza-lyrics</t>
         </is>
       </c>
-      <c r="F107" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=YrN5Z-Aj3QE</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
         <is>
           <t>Hector Acosta “El Torito”</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="C109" t="inlineStr">
         <is>
           <t>Con que ojos</t>
         </is>
       </c>
-      <c r="D108" s="2" t="inlineStr">
+      <c r="D109" s="2" t="inlineStr">
         <is>
           <t>2 Contributors
 Con que ojos Lyrics
@@ -9568,34 +10178,39 @@
 Mi cara es un mar de llanto y mi corazon un dia sin sol</t>
         </is>
       </c>
-      <c r="E108" t="inlineStr">
+      <c r="E109" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-el-torito-con-que-ojos-lyrics</t>
         </is>
       </c>
-      <c r="F108" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=M3_4mbL2u4A</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
         <is>
           <t>Hector Acosta</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="C110" t="inlineStr">
         <is>
           <t>Amorcito Enfermito</t>
         </is>
       </c>
-      <c r="D109" s="2" t="inlineStr">
+      <c r="D110" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Amorcito Enfermito Lyrics
@@ -9635,34 +10250,39 @@
 Se murió</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E110" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-amorcito-enfermito-lyrics</t>
         </is>
       </c>
-      <c r="F109" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=RfTcYeNdZHY</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
         <is>
           <t>Fernando Villalona</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr">
+      <c r="C111" t="inlineStr">
         <is>
           <t>Carnaval</t>
         </is>
       </c>
-      <c r="D110" s="2" t="inlineStr">
+      <c r="D111" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Carnaval Lyrics
@@ -9686,34 +10306,39 @@
 Pedazos de mí, tirados en el camino</t>
         </is>
       </c>
-      <c r="E110" t="inlineStr">
+      <c r="E111" t="inlineStr">
         <is>
           <t>https://genius.com/Fernando-villalona-carnaval-lyrics</t>
         </is>
       </c>
-      <c r="F110" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=VzvkapShQmY</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
         <is>
           <t>Fernando Villalona</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr">
+      <c r="C112" t="inlineStr">
         <is>
           <t>Fernando Villalona-Te Amo Demasiado</t>
         </is>
       </c>
-      <c r="D111" s="2" t="inlineStr">
+      <c r="D112" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Fernando Villalona-Te Amo Demasiado Lyrics
@@ -9751,34 +10376,39 @@
 Ya pueda olvidarte</t>
         </is>
       </c>
-      <c r="E111" t="inlineStr">
+      <c r="E112" t="inlineStr">
         <is>
           <t>https://genius.com/Fernando-villalona-fernando-villalona-te-amo-demasiado-lyrics</t>
         </is>
       </c>
-      <c r="F111" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=ShqQbwQUnLo</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
         <is>
           <t>Fernando Villalona</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
+      <c r="C113" t="inlineStr">
         <is>
           <t>Celos</t>
         </is>
       </c>
-      <c r="D112" s="2" t="inlineStr">
+      <c r="D113" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Celos Lyrics
@@ -9800,34 +10430,39 @@
 Si de ti no vivo enamorado</t>
         </is>
       </c>
-      <c r="E112" t="inlineStr">
+      <c r="E113" t="inlineStr">
         <is>
           <t>https://genius.com/Fernando-villalona-celos-lyrics</t>
         </is>
       </c>
-      <c r="F112" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=PVUVc_R1xmc</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
+      <c r="C114" t="inlineStr">
         <is>
           <t>Ni Tu Ni Yo</t>
         </is>
       </c>
-      <c r="D113" s="2" t="inlineStr">
+      <c r="D114" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Ni Tu Ni Yo Lyrics
@@ -9880,34 +10515,39 @@
 Kn00ty</t>
         </is>
       </c>
-      <c r="E113" t="inlineStr">
+      <c r="E114" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-ni-tu-ni-yo-lyrics</t>
         </is>
       </c>
-      <c r="F113" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=tjd7Y01T5Hg</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
         <is>
           <t>Sergio Vargas</t>
         </is>
       </c>
-      <c r="C114" t="inlineStr">
+      <c r="C115" t="inlineStr">
         <is>
           <t>Procuro Olvidarte</t>
         </is>
       </c>
-      <c r="D114" s="2" t="inlineStr">
+      <c r="D115" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Procuro Olvidarte Lyrics
@@ -9976,34 +10616,39 @@
 Y comprarte los meresteres toditico nuevo</t>
         </is>
       </c>
-      <c r="E114" t="inlineStr">
+      <c r="E115" t="inlineStr">
         <is>
           <t>https://genius.com/Sergio-vargas-procuro-olvidarte-lyrics</t>
         </is>
       </c>
-      <c r="F114" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=2mVIw32kJY4</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
         <is>
           <t>Hector Acosta “El Torito”</t>
         </is>
       </c>
-      <c r="C115" t="inlineStr">
+      <c r="C116" t="inlineStr">
         <is>
           <t>Aprendere</t>
         </is>
       </c>
-      <c r="D115" s="2" t="inlineStr">
+      <c r="D116" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Aprendere Lyrics
@@ -10036,34 +10681,39 @@
 Sacarlo corazon</t>
         </is>
       </c>
-      <c r="E115" t="inlineStr">
+      <c r="E116" t="inlineStr">
         <is>
           <t>https://genius.com/Hector-acosta-el-torito-aprendere-lyrics</t>
         </is>
       </c>
-      <c r="F115" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=CQbN_aTxfGc</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C116" t="inlineStr">
+      <c r="C117" t="inlineStr">
         <is>
           <t>La Mamá de la Mamá (Remix)</t>
         </is>
       </c>
-      <c r="D116" s="2" t="inlineStr">
+      <c r="D117" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">12 Contributors
 La Mamá de la Mamá  Lyrics
@@ -10225,34 +10875,39 @@
 ¡Cha-el! </t>
         </is>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="E117" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-busta-rhymes-and-anitta-la-mama-de-la-mama-remix-lyrics</t>
         </is>
       </c>
-      <c r="F116" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=D5yqLdjNyMU</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C117" t="inlineStr">
+      <c r="C118" t="inlineStr">
         <is>
           <t>Gogo Dance</t>
         </is>
       </c>
-      <c r="D117" s="2" t="inlineStr">
+      <c r="D118" s="2" t="inlineStr">
         <is>
           <t>6 Contributors
 Gogo Dance Lyrics
@@ -10328,34 +10983,39 @@
 Tirándolo' pa' arriba pa' que baile' gogo dance</t>
         </is>
       </c>
-      <c r="E117" t="inlineStr">
+      <c r="E118" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-gogo-dance-lyrics</t>
         </is>
       </c>
-      <c r="F117" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=wVib5FsxtMQ</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C118" t="inlineStr">
+      <c r="C119" t="inlineStr">
         <is>
           <t>Suave (Remix)</t>
         </is>
       </c>
-      <c r="D118" s="2" t="inlineStr">
+      <c r="D119" s="2" t="inlineStr">
         <is>
           <t>29 Contributors
 Suave  Lyrics
@@ -10627,34 +11287,39 @@
 , suave</t>
         </is>
       </c>
-      <c r="E118" t="inlineStr">
+      <c r="E119" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-suave-remix-lyrics</t>
         </is>
       </c>
-      <c r="F118" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=SpRpfev01n0</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C119" t="inlineStr">
+      <c r="C120" t="inlineStr">
         <is>
           <t>Banda De Camión</t>
         </is>
       </c>
-      <c r="D119" s="2" t="inlineStr">
+      <c r="D120" s="2" t="inlineStr">
         <is>
           <t>7 Contributors
 Banda De Camión Lyrics
@@ -10737,34 +11402,39 @@
 Ofrécome</t>
         </is>
       </c>
-      <c r="E119" t="inlineStr">
+      <c r="E120" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-banda-de-camion-lyrics</t>
         </is>
       </c>
-      <c r="F119" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=dSA9245tJPk</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C120" t="inlineStr">
+      <c r="C121" t="inlineStr">
         <is>
           <t>Singapur</t>
         </is>
       </c>
-      <c r="D120" s="2" t="inlineStr">
+      <c r="D121" s="2" t="inlineStr">
         <is>
           <t>10 Contributors
 Singapur Lyrics
@@ -10855,34 +11525,39 @@
 Yao</t>
         </is>
       </c>
-      <c r="E120" t="inlineStr">
+      <c r="E121" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-and-chael-produciendo-singapur-lyrics</t>
         </is>
       </c>
-      <c r="F120" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=N23QQV_qcV0</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
         <is>
           <t>Don Miguelo</t>
         </is>
       </c>
-      <c r="C121" t="inlineStr">
+      <c r="C122" t="inlineStr">
         <is>
           <t>El Mario de Tu Mujer</t>
         </is>
       </c>
-      <c r="D121" s="2" t="inlineStr">
+      <c r="D122" s="2" t="inlineStr">
         <is>
           <t>9 Contributors
 El Mario de Tu Mujer Lyrics
@@ -11000,34 +11675,39 @@
 Club, club, club, club</t>
         </is>
       </c>
-      <c r="E121" t="inlineStr">
+      <c r="E122" t="inlineStr">
         <is>
           <t>https://genius.com/Don-miguelo-el-mario-de-tu-mujer-lyrics</t>
         </is>
       </c>
-      <c r="F121" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=W4HjYteQFl8</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
         <is>
           <t>Pitbull</t>
         </is>
       </c>
-      <c r="C122" t="inlineStr">
+      <c r="C123" t="inlineStr">
         <is>
           <t>Como Yo Le Doy</t>
         </is>
       </c>
-      <c r="D122" s="2" t="inlineStr">
+      <c r="D123" s="2" t="inlineStr">
         <is>
           <t>14 Contributors
 Como Yo Le Doy Lyrics
@@ -11125,34 +11805,39 @@
 Dice que soy su pana, que le quita las gana'</t>
         </is>
       </c>
-      <c r="E122" t="inlineStr">
+      <c r="E123" t="inlineStr">
         <is>
           <t>https://genius.com/Pitbull-como-yo-le-doy-lyrics</t>
         </is>
       </c>
-      <c r="F122" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=zCB8Z_fO2Yo</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
         <is>
           <t>Rochy RD</t>
         </is>
       </c>
-      <c r="C123" t="inlineStr">
+      <c r="C124" t="inlineStr">
         <is>
           <t>Uva Bombom</t>
         </is>
       </c>
-      <c r="D123" s="2" t="inlineStr">
+      <c r="D124" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 Uva Bombom Lyrics
@@ -11259,34 +11944,39 @@
 Móntala, súbela</t>
         </is>
       </c>
-      <c r="E123" t="inlineStr">
+      <c r="E124" t="inlineStr">
         <is>
           <t>https://genius.com/Rochy-rd-uva-bombom-lyrics</t>
         </is>
       </c>
-      <c r="F123" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=lsEqmtE9UA0</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
         <is>
           <t>Rochy RD</t>
         </is>
       </c>
-      <c r="C124" t="inlineStr">
+      <c r="C125" t="inlineStr">
         <is>
           <t>Alta Gama</t>
         </is>
       </c>
-      <c r="D124" s="2" t="inlineStr">
+      <c r="D125" s="2" t="inlineStr">
         <is>
           <t>1 Contributor
 Alta Gama Lyrics
@@ -11377,34 +12067,39 @@
 Leo, ¡clu!, vámono'</t>
         </is>
       </c>
-      <c r="E124" t="inlineStr">
+      <c r="E125" t="inlineStr">
         <is>
           <t>https://genius.com/Rochy-rd-alta-gama-lyrics</t>
         </is>
       </c>
-      <c r="F124" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=UJLOiE8hb24</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
         <is>
           <t>Rochy RD</t>
         </is>
       </c>
-      <c r="C125" t="inlineStr">
+      <c r="C126" t="inlineStr">
         <is>
           <t>Millonario Real</t>
         </is>
       </c>
-      <c r="D125" s="2" t="inlineStr">
+      <c r="D126" s="2" t="inlineStr">
         <is>
           <t>3 Contributors
 Millonario Real Lyrics
@@ -11490,34 +12185,39 @@
 Que viene el jefe</t>
         </is>
       </c>
-      <c r="E125" t="inlineStr">
+      <c r="E126" t="inlineStr">
         <is>
           <t>https://genius.com/Rochy-rd-millonario-real-lyrics</t>
         </is>
       </c>
-      <c r="F125" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=7JvYFgVKh2o</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
         <is>
           <t>Rochy RD</t>
         </is>
       </c>
-      <c r="C126" t="inlineStr">
+      <c r="C127" t="inlineStr">
         <is>
           <t>Ella No Es Tuya (Remix)</t>
         </is>
       </c>
-      <c r="D126" s="2" t="inlineStr">
+      <c r="D127" s="2" t="inlineStr">
         <is>
           <t>7 Contributors
 Ella No Es Tuya  Lyrics
@@ -11686,34 +12386,39 @@
 )</t>
         </is>
       </c>
-      <c r="E126" t="inlineStr">
+      <c r="E127" t="inlineStr">
         <is>
           <t>https://genius.com/Rochy-rd-myke-towers-and-nicki-nicole-ella-no-es-tuya-remix-lyrics</t>
         </is>
       </c>
-      <c r="F126" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=37tmRDUK0FM</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
         <is>
           <t>El Alfa</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr">
+      <c r="C128" t="inlineStr">
         <is>
           <t>Probadita</t>
         </is>
       </c>
-      <c r="D127" s="2" t="inlineStr">
+      <c r="D128" s="2" t="inlineStr">
         <is>
           <t>4 Contributors
 Probadita Lyrics
@@ -11766,12 +12471,17 @@
 Tú te quedaste con las gana', con los deseo', y con la cosquillita</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr">
+      <c r="E128" t="inlineStr">
         <is>
           <t>https://genius.com/El-alfa-and-lenier-probadita-lyrics</t>
         </is>
       </c>
-      <c r="F127" t="inlineStr">
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=RTmJP34CPC8</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>

</xml_diff>